<commit_message>
Updated demo notebooks to incorporate change of ppm to res
Tested old notebooks to make sure nothing changed while implementing
new algo
</commit_message>
<xml_diff>
--- a/Demo/auto_detect_dual_label_isotope_res293808_at307_orbitrap.xlsx
+++ b/Demo/auto_detect_dual_label_isotope_res293808_at307_orbitrap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/Documents/NA_Correction/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E45C0C-BBB2-744B-959B-B34D385C4D0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB71B7-9A9D-2F4F-9FC6-EB5C45A88E1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,21 +641,18 @@
             <v>Unlabeled Fragment</v>
           </cell>
           <cell r="H1" t="str">
-            <v>Indistinguishable_isotope</v>
+            <v>NA Corrected</v>
           </cell>
           <cell r="I1" t="str">
-            <v>NA Corrected</v>
+            <v>Intensity_y</v>
           </cell>
           <cell r="J1" t="str">
-            <v>Intensity_y</v>
+            <v>NA Corrected with zero</v>
           </cell>
           <cell r="K1" t="str">
-            <v>NA Corrected with zero</v>
+            <v>Pool_total</v>
           </cell>
           <cell r="L1" t="str">
-            <v>Pool_total</v>
-          </cell>
-          <cell r="M1" t="str">
             <v>Fractional enrichment</v>
           </cell>
         </row>
@@ -675,23 +672,20 @@
           <cell r="G2" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H2" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H2">
+            <v>-1.9964753016790599E-16</v>
           </cell>
           <cell r="I2">
-            <v>9.8699999999999994E-17</v>
+            <v>0</v>
           </cell>
           <cell r="J2">
             <v>0</v>
           </cell>
           <cell r="K2">
-            <v>9.8699999999999994E-17</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L2">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M2">
-            <v>9.6399999999999999E-17</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="3">
@@ -710,23 +704,20 @@
           <cell r="G3" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H3" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H3">
+            <v>2.1634941269091599E-17</v>
           </cell>
           <cell r="I3">
-            <v>6.48E-17</v>
+            <v>0</v>
           </cell>
           <cell r="J3">
-            <v>0</v>
+            <v>2.1634941269091599E-17</v>
           </cell>
           <cell r="K3">
-            <v>6.48E-17</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L3">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M3">
-            <v>6.3300000000000001E-17</v>
+            <v>1.9629480568110799E-17</v>
           </cell>
         </row>
         <row r="4">
@@ -745,23 +736,20 @@
           <cell r="G4" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H4" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H4">
+            <v>1.6760988139682E-16</v>
           </cell>
           <cell r="I4">
-            <v>2.1899999999999999E-17</v>
+            <v>0</v>
           </cell>
           <cell r="J4">
-            <v>0</v>
+            <v>1.6760988139682E-16</v>
           </cell>
           <cell r="K4">
-            <v>2.1899999999999999E-17</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L4">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M4">
-            <v>2.14E-17</v>
+            <v>1.5207320736306199E-16</v>
           </cell>
         </row>
         <row r="5">
@@ -780,23 +768,20 @@
           <cell r="G5" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H5" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H5">
+            <v>0.22301946992437999</v>
           </cell>
           <cell r="I5">
-            <v>0.20777352599999999</v>
+            <v>0.17799999999999999</v>
           </cell>
           <cell r="J5">
-            <v>0.17799999999999999</v>
+            <v>0.22301946992437999</v>
           </cell>
           <cell r="K5">
-            <v>0.20777352599999999</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L5">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M5">
-            <v>0.202971613</v>
+            <v>0.202346578931795</v>
           </cell>
         </row>
         <row r="6">
@@ -815,22 +800,19 @@
           <cell r="G6" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H6" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H6">
+            <v>-1.2214701192655799E-3</v>
           </cell>
           <cell r="I6">
-            <v>-1.6322730000000001E-3</v>
+            <v>1.2999999999999999E-2</v>
           </cell>
           <cell r="J6">
-            <v>1.2999999999999999E-2</v>
+            <v>0</v>
           </cell>
           <cell r="K6">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L6">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M6">
             <v>0</v>
           </cell>
         </row>
@@ -850,22 +832,19 @@
           <cell r="G7" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H7" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H7">
+            <v>-9.9846063953359897E-3</v>
           </cell>
           <cell r="I7">
-            <v>-2.3560200000000001E-4</v>
+            <v>2.0000000000000001E-4</v>
           </cell>
           <cell r="J7">
-            <v>2.0000000000000001E-4</v>
+            <v>0</v>
           </cell>
           <cell r="K7">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L7">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M7">
             <v>0</v>
           </cell>
         </row>
@@ -885,23 +864,20 @@
           <cell r="G8" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H8" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H8">
+            <v>-3.6122906621732201E-5</v>
           </cell>
           <cell r="I8">
-            <v>1.18535E-4</v>
+            <v>1E-4</v>
           </cell>
           <cell r="J8">
-            <v>1E-4</v>
+            <v>0</v>
           </cell>
           <cell r="K8">
-            <v>1.18535E-4</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L8">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M8">
-            <v>1.15795E-4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="9">
@@ -920,23 +896,20 @@
           <cell r="G9" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H9" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H9">
+            <v>2.6399907104614202E-3</v>
           </cell>
           <cell r="I9">
-            <v>5.2849699999999995E-4</v>
+            <v>7.85E-2</v>
           </cell>
           <cell r="J9">
-            <v>7.85E-2</v>
+            <v>2.6399907104614202E-3</v>
           </cell>
           <cell r="K9">
-            <v>5.2849699999999995E-4</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L9">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M9">
-            <v>5.1628199999999996E-4</v>
+            <v>2.3952755732704299E-3</v>
           </cell>
         </row>
         <row r="10">
@@ -955,22 +928,19 @@
           <cell r="G10" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H10" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H10">
+            <v>-9.7559887392098504E-19</v>
           </cell>
           <cell r="I10">
-            <v>-1.31E-7</v>
+            <v>0</v>
           </cell>
           <cell r="J10">
             <v>0</v>
           </cell>
           <cell r="K10">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L10">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M10">
             <v>0</v>
           </cell>
         </row>
@@ -990,23 +960,20 @@
           <cell r="G11" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H11" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H11">
+            <v>-2.6128393452825798E-19</v>
           </cell>
           <cell r="I11">
-            <v>9.4000000000000006E-10</v>
+            <v>0</v>
           </cell>
           <cell r="J11">
             <v>0</v>
           </cell>
           <cell r="K11">
-            <v>9.4000000000000006E-10</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L11">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M11">
-            <v>9.1900000000000003E-10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="12">
@@ -1025,23 +992,20 @@
           <cell r="G12" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H12" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H12">
+            <v>6.8876597725337701E-18</v>
           </cell>
           <cell r="I12">
-            <v>4.9300000000000001E-9</v>
+            <v>0</v>
           </cell>
           <cell r="J12">
-            <v>0</v>
+            <v>6.8876597725337701E-18</v>
           </cell>
           <cell r="K12">
-            <v>4.9300000000000001E-9</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L12">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M12">
-            <v>4.8099999999999997E-9</v>
+            <v>6.2492050236282797E-18</v>
           </cell>
         </row>
         <row r="13">
@@ -1060,23 +1024,20 @@
           <cell r="G13" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H13" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H13">
+            <v>-3.7293959749569602E-2</v>
           </cell>
           <cell r="I13">
-            <v>7.2590199999999995E-4</v>
+            <v>4.7000000000000002E-3</v>
           </cell>
           <cell r="J13">
-            <v>4.7000000000000002E-3</v>
+            <v>0</v>
           </cell>
           <cell r="K13">
-            <v>7.2590199999999995E-4</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L13">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M13">
-            <v>7.0912600000000003E-4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="14">
@@ -1095,22 +1056,19 @@
           <cell r="G14" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H14" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H14">
+            <v>-4.1115769241794199E-4</v>
           </cell>
           <cell r="I14">
-            <v>-3.8299599999999998E-4</v>
+            <v>1.6000000000000001E-3</v>
           </cell>
           <cell r="J14">
-            <v>1.6000000000000001E-3</v>
+            <v>0</v>
           </cell>
           <cell r="K14">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L14">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M14">
             <v>0</v>
           </cell>
         </row>
@@ -1130,23 +1088,20 @@
           <cell r="G15" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H15" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H15">
+            <v>1.4317297021819201E-3</v>
           </cell>
           <cell r="I15">
-            <v>1.331186E-3</v>
+            <v>9.1000000000000004E-3</v>
           </cell>
           <cell r="J15">
-            <v>9.1000000000000004E-3</v>
+            <v>1.4317297021819201E-3</v>
           </cell>
           <cell r="K15">
-            <v>1.331186E-3</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L15">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M15">
-            <v>1.30042E-3</v>
+            <v>1.29901486757985E-3</v>
           </cell>
         </row>
         <row r="16">
@@ -1165,22 +1120,19 @@
           <cell r="G16" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H16" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H16">
+            <v>-1.2793322671959199E-3</v>
           </cell>
           <cell r="I16">
-            <v>-3.00081E-4</v>
+            <v>0</v>
           </cell>
           <cell r="J16">
             <v>0</v>
           </cell>
           <cell r="K16">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L16">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M16">
             <v>0</v>
           </cell>
         </row>
@@ -1200,23 +1152,20 @@
           <cell r="G17" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H17" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H17">
+            <v>3.5181002638137498E-4</v>
           </cell>
           <cell r="I17">
-            <v>3.2866699999999999E-4</v>
+            <v>4.0000000000000002E-4</v>
           </cell>
           <cell r="J17">
-            <v>4.0000000000000002E-4</v>
+            <v>3.5181002638137498E-4</v>
           </cell>
           <cell r="K17">
-            <v>3.2866699999999999E-4</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L17">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M17">
-            <v>3.2107099999999998E-4</v>
+            <v>3.19198836300317E-4</v>
           </cell>
         </row>
         <row r="18">
@@ -1235,23 +1184,20 @@
           <cell r="G18" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H18" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H18">
+            <v>3.3179111185479303E-5</v>
           </cell>
           <cell r="I18">
-            <v>2.7699999999999999E-5</v>
+            <v>6.9999999999999999E-4</v>
           </cell>
           <cell r="J18">
-            <v>6.9999999999999999E-4</v>
+            <v>3.3179111185479303E-5</v>
           </cell>
           <cell r="K18">
-            <v>2.7699999999999999E-5</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L18">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M18">
-            <v>2.6999999999999999E-5</v>
+            <v>3.0103558414230901E-5</v>
           </cell>
         </row>
         <row r="19">
@@ -1270,23 +1216,20 @@
           <cell r="G19" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H19" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H19">
+            <v>1.6076528420901899E-3</v>
           </cell>
           <cell r="I19">
-            <v>-2.4499999999999998E-6</v>
+            <v>0</v>
           </cell>
           <cell r="J19">
-            <v>0</v>
+            <v>1.6076528420901899E-3</v>
           </cell>
           <cell r="K19">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L19">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M19">
-            <v>0</v>
+            <v>1.4586307321832899E-3</v>
           </cell>
         </row>
         <row r="20">
@@ -1305,22 +1248,19 @@
           <cell r="G20" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H20" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H20">
+            <v>-7.0677771231308196E-6</v>
           </cell>
           <cell r="I20">
-            <v>-2.41E-5</v>
+            <v>0</v>
           </cell>
           <cell r="J20">
             <v>0</v>
           </cell>
           <cell r="K20">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L20">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M20">
             <v>0</v>
           </cell>
         </row>
@@ -1340,23 +1280,20 @@
           <cell r="G21" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H21" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H21">
+            <v>9.2714091962434298E-5</v>
           </cell>
           <cell r="I21">
-            <v>9.3399999999999997E-7</v>
+            <v>0</v>
           </cell>
           <cell r="J21">
-            <v>0</v>
+            <v>9.2714091962434298E-5</v>
           </cell>
           <cell r="K21">
-            <v>9.3399999999999997E-7</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L21">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M21">
-            <v>9.1200000000000001E-7</v>
+            <v>8.4119917125296401E-5</v>
           </cell>
         </row>
         <row r="22">
@@ -1375,22 +1312,19 @@
           <cell r="G22" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H22" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H22">
+            <v>-1.5507671251513899E-5</v>
           </cell>
           <cell r="I22">
-            <v>-4.6499999999999999E-7</v>
+            <v>0</v>
           </cell>
           <cell r="J22">
             <v>0</v>
           </cell>
           <cell r="K22">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L22">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M22">
             <v>0</v>
           </cell>
         </row>
@@ -1410,22 +1344,19 @@
           <cell r="G23" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H23" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H23">
+            <v>-6.8345565761581705E-5</v>
           </cell>
           <cell r="I23">
-            <v>-1.6199999999999999E-8</v>
+            <v>0</v>
           </cell>
           <cell r="J23">
             <v>0</v>
           </cell>
           <cell r="K23">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L23">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M23">
             <v>0</v>
           </cell>
         </row>
@@ -1445,23 +1376,20 @@
           <cell r="G24" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H24" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H24">
+            <v>-3.3380773033735899E-16</v>
           </cell>
           <cell r="I24">
-            <v>3.3100000000000001E-6</v>
+            <v>0</v>
           </cell>
           <cell r="J24">
             <v>0</v>
           </cell>
           <cell r="K24">
-            <v>3.3100000000000001E-6</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L24">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M24">
-            <v>3.2399999999999999E-6</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="25">
@@ -1480,22 +1408,19 @@
           <cell r="G25" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H25" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H25">
+            <v>-1.3764222830651901E-16</v>
           </cell>
           <cell r="I25">
-            <v>-2.3800000000000001E-8</v>
+            <v>0</v>
           </cell>
           <cell r="J25">
             <v>0</v>
           </cell>
           <cell r="K25">
-            <v>0</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L25">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M25">
             <v>0</v>
           </cell>
         </row>
@@ -1515,23 +1440,20 @@
           <cell r="G26" t="str">
             <v>Glutathione</v>
           </cell>
-          <cell r="H26" t="str">
-            <v>{'C': ['O17'], 'N': ['S34']}</v>
+          <cell r="H26">
+            <v>0.872542017953719</v>
           </cell>
           <cell r="I26">
-            <v>0.81281945600000005</v>
+            <v>0.68079999999999996</v>
           </cell>
           <cell r="J26">
-            <v>0.68079999999999996</v>
+            <v>0.872542017953719</v>
           </cell>
           <cell r="K26">
-            <v>0.81281945600000005</v>
+            <v>1.10216575492266</v>
           </cell>
           <cell r="L26">
-            <v>1.023658051</v>
-          </cell>
-          <cell r="M26">
-            <v>0.79403415499999996</v>
+            <v>0.79166133955499496</v>
           </cell>
         </row>
       </sheetData>
@@ -1840,7 +1762,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1867,8 +1789,8 @@
         <v>0.8</v>
       </c>
       <c r="C2">
-        <f>VLOOKUP(A2,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>0.79403415499999996</v>
+        <f>VLOOKUP(A2,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>0.79166133955499496</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1879,8 +1801,8 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <f>VLOOKUP(A3,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>0.202971613</v>
+        <f>VLOOKUP(A3,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>0.202346578931795</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1891,8 +1813,8 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f>VLOOKUP(A4,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>1.30042E-3</v>
+        <f>VLOOKUP(A4,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>1.29901486757985E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1903,8 +1825,8 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f>VLOOKUP(A5,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>7.0912600000000003E-4</v>
+        <f>VLOOKUP(A5,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1915,8 +1837,8 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>VLOOKUP(A6,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>5.1628199999999996E-4</v>
+        <f>VLOOKUP(A6,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>2.3952755732704299E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1927,8 +1849,8 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>VLOOKUP(A7,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>3.2107099999999998E-4</v>
+        <f>VLOOKUP(A7,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>3.19198836300317E-4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1939,8 +1861,8 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>VLOOKUP(A8,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>1.15795E-4</v>
+        <f>VLOOKUP(A8,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1951,8 +1873,8 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>VLOOKUP(A9,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>2.6999999999999999E-5</v>
+        <f>VLOOKUP(A9,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>3.0103558414230901E-5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1963,8 +1885,8 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>VLOOKUP(A10,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
-        <v>3.2399999999999999E-6</v>
+        <f>VLOOKUP(A10,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1975,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>VLOOKUP(A11,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
+        <f>VLOOKUP(A11,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -1987,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>VLOOKUP(A12,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
+        <f>VLOOKUP(A12,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -1999,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>VLOOKUP(A13,[1]auto_detect_dual_label_isotope_!$C:$M,11,FALSE)</f>
+        <f>VLOOKUP(A13,[1]auto_detect_dual_label_isotope_!$C:$M,10,FALSE)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>